<commit_message>
🚀 WORKING BUILD: Fixed file corruption and syntax errors
✅ Resolved BessQuoteBuilder.tsx corruption
✅ Fixed incomplete TextRun statements
✅ Removed duplicate lines and added missing commas
✅ Build successfully completed (1675 modules)
✅ All components compiling properly
✅ UserProfile integration ready
✅ Export functionality restored

- Fixed line 1035 broken new Text statement
- Removed duplicate TableCell at line 1036
- Added proper comma syntax for table structure
- Maintained all existing features and UI components
- Ready for additional feature development
</commit_message>
<xml_diff>
--- a/server/templates/BESS_Quote_Template.xlsx
+++ b/server/templates/BESS_Quote_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertchristopher/merlin/server/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC4DA25B-4EE2-044B-B080-51ACD7A1D3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2487F4-70A8-4742-AF4D-B7C6F1414A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="540" windowWidth="24460" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="540" windowWidth="24460" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BESS Calculator" sheetId="1" r:id="rId1"/>
@@ -892,7 +892,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1577,7 +1577,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>